<commit_message>
update go.mod and packages name
</commit_message>
<xml_diff>
--- a/data/excel/2023/05/17.xlsx
+++ b/data/excel/2023/05/17.xlsx
@@ -34,6 +34,9 @@
     <t>Avg Price</t>
   </si>
   <si>
+    <t>50.00</t>
+  </si>
+  <si>
     <t>55.00</t>
   </si>
   <si>
@@ -49,18 +52,15 @@
     <t>60.00</t>
   </si>
   <si>
-    <t>50.00</t>
+    <t>70.00</t>
+  </si>
+  <si>
+    <t>65.00</t>
   </si>
   <si>
     <t>Tomato Big(Indian)</t>
   </si>
   <si>
-    <t>70.00</t>
-  </si>
-  <si>
-    <t>65.00</t>
-  </si>
-  <si>
     <t>Tomato Small(Local)</t>
   </si>
   <si>
@@ -73,13 +73,16 @@
     <t>28.00</t>
   </si>
   <si>
+    <t>Tomato Small(Tunnel)</t>
+  </si>
+  <si>
+    <t>40.00</t>
+  </si>
+  <si>
     <t>45.00</t>
   </si>
   <si>
-    <t>Tomato Small(Tunnel)</t>
-  </si>
-  <si>
-    <t>40.00</t>
+    <t>Tomato Small(Indian)</t>
   </si>
   <si>
     <t>35.00</t>
@@ -88,21 +91,18 @@
     <t>37.50</t>
   </si>
   <si>
-    <t>Tomato Small(Indian)</t>
-  </si>
-  <si>
     <t>Tomato Small(Terai)</t>
   </si>
   <si>
+    <t>34.60</t>
+  </si>
+  <si>
+    <t>Potato Red</t>
+  </si>
+  <si>
     <t>34.00</t>
   </si>
   <si>
-    <t>34.60</t>
-  </si>
-  <si>
-    <t>Potato Red</t>
-  </si>
-  <si>
     <t>Potato Red(Indian)</t>
   </si>
   <si>
@@ -112,18 +112,18 @@
     <t>30.67</t>
   </si>
   <si>
+    <t>26.00</t>
+  </si>
+  <si>
+    <t>26.67</t>
+  </si>
+  <si>
+    <t>Potato White</t>
+  </si>
+  <si>
     <t>27.00</t>
   </si>
   <si>
-    <t>26.00</t>
-  </si>
-  <si>
-    <t>26.67</t>
-  </si>
-  <si>
-    <t>Potato White</t>
-  </si>
-  <si>
     <t>Onion Dry (Indian)</t>
   </si>
   <si>
@@ -133,6 +133,9 @@
     <t>Carrot(Local)</t>
   </si>
   <si>
+    <t>11.80</t>
+  </si>
+  <si>
     <t>Cabbage(Local)</t>
   </si>
   <si>
@@ -142,9 +145,6 @@
     <t>10.00</t>
   </si>
   <si>
-    <t>11.80</t>
-  </si>
-  <si>
     <t>Cauli Local</t>
   </si>
   <si>
@@ -157,21 +157,21 @@
     <t>Raddish Red</t>
   </si>
   <si>
+    <t>20.00</t>
+  </si>
+  <si>
     <t>22.50</t>
   </si>
   <si>
     <t>Raddish White(Local)</t>
   </si>
   <si>
-    <t>20.00</t>
+    <t>27.50</t>
   </si>
   <si>
     <t>Raddish White(Hybrid)</t>
   </si>
   <si>
-    <t>27.50</t>
-  </si>
-  <si>
     <t>Brinjal Long</t>
   </si>
   <si>
@@ -181,13 +181,16 @@
     <t>Cow pea(Long)</t>
   </si>
   <si>
+    <t>76.67</t>
+  </si>
+  <si>
     <t>Cowpea(Short)</t>
   </si>
   <si>
     <t>80.00</t>
   </si>
   <si>
-    <t>76.67</t>
+    <t>Green Peas</t>
   </si>
   <si>
     <t>140.00</t>
@@ -199,24 +202,21 @@
     <t>136.67</t>
   </si>
   <si>
-    <t>Green Peas</t>
-  </si>
-  <si>
     <t>French Bean(Local)</t>
   </si>
   <si>
     <t>75.00</t>
   </si>
   <si>
+    <t>90.00</t>
+  </si>
+  <si>
     <t>86.67</t>
   </si>
   <si>
     <t>French Bean(Hybrid)</t>
   </si>
   <si>
-    <t>90.00</t>
-  </si>
-  <si>
     <t>French Bean(Rajma)</t>
   </si>
   <si>
@@ -241,12 +241,12 @@
     <t>Bitter Gourd</t>
   </si>
   <si>
+    <t>56.00</t>
+  </si>
+  <si>
     <t>Bottle Gourd</t>
   </si>
   <si>
-    <t>56.00</t>
-  </si>
-  <si>
     <t>95.00</t>
   </si>
   <si>
@@ -295,12 +295,12 @@
     <t>Barela</t>
   </si>
   <si>
+    <t>Christophine</t>
+  </si>
+  <si>
     <t>46.67</t>
   </si>
   <si>
-    <t>Christophine</t>
-  </si>
-  <si>
     <t>Brd Leaf Mustard</t>
   </si>
   <si>
@@ -370,27 +370,27 @@
     <t>Knolkhol</t>
   </si>
   <si>
+    <t>200.00</t>
+  </si>
+  <si>
+    <t>150.00</t>
+  </si>
+  <si>
     <t>183.33</t>
   </si>
   <si>
     <t>Celery</t>
   </si>
   <si>
-    <t>200.00</t>
-  </si>
-  <si>
-    <t>150.00</t>
-  </si>
-  <si>
     <t>Parseley</t>
   </si>
   <si>
+    <t>Fennel Leaf</t>
+  </si>
+  <si>
     <t>115.00</t>
   </si>
   <si>
-    <t>Fennel Leaf</t>
-  </si>
-  <si>
     <t>Mint</t>
   </si>
   <si>
@@ -400,12 +400,12 @@
     <t>Turnip A</t>
   </si>
   <si>
+    <t>146.67</t>
+  </si>
+  <si>
     <t>Tamarind</t>
   </si>
   <si>
-    <t>146.67</t>
-  </si>
-  <si>
     <t>Bamboo Shoot</t>
   </si>
   <si>
@@ -415,12 +415,12 @@
     <t>Tofu</t>
   </si>
   <si>
+    <t>283.33</t>
+  </si>
+  <si>
     <t>Gundruk</t>
   </si>
   <si>
-    <t>283.33</t>
-  </si>
-  <si>
     <t>Apple(Fuji)</t>
   </si>
   <si>
@@ -439,21 +439,21 @@
     <t>210.00</t>
   </si>
   <si>
+    <t>Pomegranate</t>
+  </si>
+  <si>
     <t>280.00</t>
   </si>
   <si>
     <t>270.00</t>
   </si>
   <si>
-    <t>Pomegranate</t>
+    <t>223.33</t>
   </si>
   <si>
     <t>Mango(Maldah)</t>
   </si>
   <si>
-    <t>223.33</t>
-  </si>
-  <si>
     <t>Mango(Dushari)</t>
   </si>
   <si>
@@ -463,30 +463,30 @@
     <t>213.33</t>
   </si>
   <si>
+    <t>335.00</t>
+  </si>
+  <si>
     <t>Grapes(Black)</t>
   </si>
   <si>
     <t>320.00</t>
   </si>
   <si>
-    <t>335.00</t>
-  </si>
-  <si>
     <t>Water Melon(Green)</t>
   </si>
   <si>
     <t>43.33</t>
   </si>
   <si>
+    <t>165.00</t>
+  </si>
+  <si>
     <t>Sweet Orange</t>
   </si>
   <si>
     <t>180.00</t>
   </si>
   <si>
-    <t>165.00</t>
-  </si>
-  <si>
     <t>Mandarin</t>
   </si>
   <si>
@@ -556,25 +556,25 @@
     <t>465.00</t>
   </si>
   <si>
+    <t>Chilli Green</t>
+  </si>
+  <si>
     <t>96.00</t>
   </si>
   <si>
-    <t>Chilli Green</t>
-  </si>
-  <si>
     <t>Chilli Green(Bullet)</t>
   </si>
   <si>
     <t>Chilli Green(Machhe)</t>
   </si>
   <si>
+    <t>Chilli Green(Akbare)</t>
+  </si>
+  <si>
     <t>400.00</t>
   </si>
   <si>
     <t>375.00</t>
-  </si>
-  <si>
-    <t>Chilli Green(Akbare)</t>
   </si>
   <si>
     <t>Capsicum</t>
@@ -954,53 +954,53 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -1014,93 +1014,93 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
         <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
         <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>26</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
         <v>30</v>
@@ -1114,39 +1114,39 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
         <v>35</v>
       </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>32</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>33</v>
-      </c>
-      <c r="F10" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
         <v>37</v>
@@ -1154,79 +1154,79 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
         <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
         <v>13</v>
-      </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" t="s">
         <v>39</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
         <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F15" t="s">
         <v>44</v>
@@ -1234,53 +1234,53 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
         <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
         <v>16</v>
@@ -1289,44 +1289,44 @@
         <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
         <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" t="s">
         <v>21</v>
-      </c>
-      <c r="F19" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
         <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F20" t="s">
         <v>44</v>
@@ -1334,79 +1334,79 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
         <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" t="s">
         <v>21</v>
-      </c>
-      <c r="F21" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" t="s">
         <v>55</v>
-      </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" t="s">
         <v>61</v>
-      </c>
-      <c r="C23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" t="s">
-        <v>59</v>
-      </c>
-      <c r="F23" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
         <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s">
         <v>63</v>
@@ -1414,33 +1414,33 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" t="s">
         <v>65</v>
-      </c>
-      <c r="C25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" t="s">
-        <v>66</v>
-      </c>
-      <c r="E25" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
         <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
         <v>68</v>
@@ -1454,13 +1454,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
         <v>73</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D27" t="s">
         <v>71</v>
@@ -1474,59 +1474,59 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
         <v>74</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F28" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" t="s">
         <v>75</v>
-      </c>
-      <c r="C29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
         <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D30" t="s">
         <v>69</v>
       </c>
       <c r="E30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F30" t="s">
         <v>77</v>
@@ -1534,19 +1534,19 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
         <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F31" t="s">
         <v>79</v>
@@ -1554,59 +1554,59 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
         <v>81</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E32" t="s">
         <v>16</v>
       </c>
       <c r="F32" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
         <v>82</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E33" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F33" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
         <v>84</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E34" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F34" t="s">
         <v>83</v>
@@ -1614,19 +1614,19 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B35" t="s">
         <v>85</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E35" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F35" t="s">
         <v>86</v>
@@ -1634,79 +1634,79 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B36" t="s">
         <v>87</v>
       </c>
       <c r="C36" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E36" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" t="s">
         <v>21</v>
-      </c>
-      <c r="F36" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
         <v>88</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" t="s">
         <v>21</v>
-      </c>
-      <c r="F37" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
         <v>89</v>
       </c>
       <c r="C38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
         <v>90</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E39" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F39" t="s">
         <v>91</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
         <v>92</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D40" t="s">
         <v>71</v>
@@ -1734,53 +1734,53 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B41" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" t="s">
         <v>94</v>
-      </c>
-      <c r="C41" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" t="s">
-        <v>21</v>
-      </c>
-      <c r="F41" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B42" t="s">
         <v>95</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F42" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
         <v>96</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D43" t="s">
         <v>71</v>
@@ -1794,13 +1794,13 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B44" t="s">
         <v>97</v>
       </c>
       <c r="C44" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D44" t="s">
         <v>71</v>
@@ -1814,33 +1814,33 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B45" t="s">
         <v>98</v>
       </c>
       <c r="C45" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F45" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B46" t="s">
         <v>99</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D46" t="s">
         <v>71</v>
@@ -1854,39 +1854,39 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B47" t="s">
         <v>100</v>
       </c>
       <c r="C47" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E47" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F47" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B48" t="s">
         <v>102</v>
       </c>
       <c r="C48" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D48" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F48" t="s">
         <v>101</v>
@@ -1894,13 +1894,13 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B49" t="s">
         <v>103</v>
       </c>
       <c r="C49" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D49" t="s">
         <v>71</v>
@@ -1914,13 +1914,13 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B50" t="s">
         <v>107</v>
       </c>
       <c r="C50" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D50" t="s">
         <v>104</v>
@@ -1934,13 +1934,13 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B51" t="s">
         <v>108</v>
       </c>
       <c r="C51" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D51" t="s">
         <v>109</v>
@@ -1954,33 +1954,33 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B52" t="s">
         <v>111</v>
       </c>
       <c r="C52" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F52" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B53" t="s">
         <v>112</v>
       </c>
       <c r="C53" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D53" t="s">
         <v>71</v>
@@ -1994,59 +1994,59 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B54" t="s">
         <v>113</v>
       </c>
       <c r="C54" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D54" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E54" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F54" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B55" t="s">
         <v>114</v>
       </c>
       <c r="C55" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D55" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F55" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B56" t="s">
         <v>115</v>
       </c>
       <c r="C56" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D56" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E56" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F56" t="s">
         <v>83</v>
@@ -2054,93 +2054,93 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B57" t="s">
         <v>116</v>
       </c>
       <c r="C57" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D57" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E57" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F57" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B58" t="s">
         <v>117</v>
       </c>
       <c r="C58" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D58" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E58" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F58" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B59" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" t="s">
+        <v>118</v>
+      </c>
+      <c r="E59" t="s">
         <v>119</v>
       </c>
-      <c r="C59" t="s">
-        <v>9</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="F59" t="s">
         <v>120</v>
-      </c>
-      <c r="E59" t="s">
-        <v>121</v>
-      </c>
-      <c r="F59" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B60" t="s">
         <v>122</v>
       </c>
       <c r="C60" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D60" t="s">
+        <v>118</v>
+      </c>
+      <c r="E60" t="s">
+        <v>119</v>
+      </c>
+      <c r="F60" t="s">
         <v>120</v>
-      </c>
-      <c r="E60" t="s">
-        <v>121</v>
-      </c>
-      <c r="F60" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C61" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D61" t="s">
         <v>71</v>
@@ -2149,24 +2149,24 @@
         <v>68</v>
       </c>
       <c r="F61" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B62" t="s">
         <v>125</v>
       </c>
       <c r="C62" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D62" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E62" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F62" t="s">
         <v>126</v>
@@ -2174,59 +2174,59 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B63" t="s">
         <v>127</v>
       </c>
       <c r="C63" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D63" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F63" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B64" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" t="s">
+        <v>119</v>
+      </c>
+      <c r="E64" t="s">
+        <v>59</v>
+      </c>
+      <c r="F64" t="s">
         <v>128</v>
-      </c>
-      <c r="C64" t="s">
-        <v>9</v>
-      </c>
-      <c r="D64" t="s">
-        <v>121</v>
-      </c>
-      <c r="E64" t="s">
-        <v>58</v>
-      </c>
-      <c r="F64" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B65" t="s">
         <v>130</v>
       </c>
       <c r="C65" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D65" t="s">
         <v>69</v>
       </c>
       <c r="E65" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F65" t="s">
         <v>131</v>
@@ -2234,13 +2234,13 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B66" t="s">
         <v>132</v>
       </c>
       <c r="C66" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D66" t="s">
         <v>71</v>
@@ -2254,13 +2254,13 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B67" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C67" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D67" t="s">
         <v>104</v>
@@ -2269,18 +2269,18 @@
         <v>105</v>
       </c>
       <c r="F67" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B68" t="s">
         <v>135</v>
       </c>
       <c r="C68" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D68" t="s">
         <v>104</v>
@@ -2289,12 +2289,12 @@
         <v>105</v>
       </c>
       <c r="F68" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B69" t="s">
         <v>136</v>
@@ -2303,30 +2303,30 @@
         <v>137</v>
       </c>
       <c r="D69" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E69" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F69" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B70" t="s">
         <v>138</v>
       </c>
       <c r="C70" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D70" t="s">
         <v>139</v>
       </c>
       <c r="E70" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F70" t="s">
         <v>140</v>
@@ -2334,79 +2334,79 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B71" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C71" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D71" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E71" t="s">
         <v>105</v>
       </c>
       <c r="F71" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B72" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C72" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D72" t="s">
         <v>105</v>
       </c>
       <c r="E72" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F72" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B73" t="s">
         <v>146</v>
       </c>
       <c r="C73" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D73" t="s">
         <v>105</v>
       </c>
       <c r="E73" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F73" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B74" t="s">
         <v>147</v>
       </c>
       <c r="C74" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D74" t="s">
         <v>139</v>
       </c>
       <c r="E74" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F74" t="s">
         <v>148</v>
@@ -2414,39 +2414,39 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B75" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C75" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D75" t="s">
         <v>109</v>
       </c>
       <c r="E75" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F75" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B76" t="s">
         <v>152</v>
       </c>
       <c r="C76" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D76" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F76" t="s">
         <v>153</v>
@@ -2454,39 +2454,39 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B77" t="s">
+        <v>155</v>
+      </c>
+      <c r="C77" t="s">
+        <v>10</v>
+      </c>
+      <c r="D77" t="s">
+        <v>156</v>
+      </c>
+      <c r="E77" t="s">
+        <v>119</v>
+      </c>
+      <c r="F77" t="s">
         <v>154</v>
-      </c>
-      <c r="C77" t="s">
-        <v>9</v>
-      </c>
-      <c r="D77" t="s">
-        <v>155</v>
-      </c>
-      <c r="E77" t="s">
-        <v>121</v>
-      </c>
-      <c r="F77" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B78" t="s">
         <v>157</v>
       </c>
       <c r="C78" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D78" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E78" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F78" t="s">
         <v>158</v>
@@ -2494,7 +2494,7 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B79" t="s">
         <v>159</v>
@@ -2503,10 +2503,10 @@
         <v>160</v>
       </c>
       <c r="D79" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E79" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F79" t="s">
         <v>161</v>
@@ -2514,19 +2514,19 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B80" t="s">
         <v>162</v>
       </c>
       <c r="C80" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D80" t="s">
         <v>69</v>
       </c>
       <c r="E80" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F80" t="s">
         <v>77</v>
@@ -2534,19 +2534,19 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B81" t="s">
         <v>163</v>
       </c>
       <c r="C81" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D81" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E81" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F81" t="s">
         <v>44</v>
@@ -2554,19 +2554,19 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B82" t="s">
         <v>165</v>
       </c>
       <c r="C82" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D82" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E82" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F82" t="s">
         <v>164</v>
@@ -2574,16 +2574,16 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B83" t="s">
         <v>166</v>
       </c>
       <c r="C83" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D83" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E83" t="s">
         <v>104</v>
@@ -2594,19 +2594,19 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B84" t="s">
         <v>168</v>
       </c>
       <c r="C84" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D84" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E84" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F84" t="s">
         <v>44</v>
@@ -2614,19 +2614,19 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B85" t="s">
         <v>169</v>
       </c>
       <c r="C85" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D85" t="s">
         <v>69</v>
       </c>
       <c r="E85" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F85" t="s">
         <v>131</v>
@@ -2634,13 +2634,13 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B86" t="s">
         <v>170</v>
       </c>
       <c r="C86" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D86" t="s">
         <v>171</v>
@@ -2654,13 +2654,13 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B87" t="s">
         <v>174</v>
       </c>
       <c r="C87" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D87" t="s">
         <v>171</v>
@@ -2674,13 +2674,13 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B88" t="s">
         <v>175</v>
       </c>
       <c r="C88" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D88" t="s">
         <v>104</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B89" t="s">
         <v>177</v>
       </c>
       <c r="C89" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D89" t="s">
         <v>178</v>
@@ -2714,39 +2714,39 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B90" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C90" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D90" t="s">
         <v>69</v>
       </c>
       <c r="E90" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F90" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B91" t="s">
         <v>182</v>
       </c>
       <c r="C91" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D91" t="s">
         <v>69</v>
       </c>
       <c r="E91" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F91" t="s">
         <v>77</v>
@@ -2754,19 +2754,19 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B92" t="s">
         <v>183</v>
       </c>
       <c r="C92" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D92" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E92" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F92" t="s">
         <v>164</v>
@@ -2774,39 +2774,39 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B93" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C93" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D93" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E93" t="s">
         <v>109</v>
       </c>
       <c r="F93" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B94" t="s">
         <v>187</v>
       </c>
       <c r="C94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D94" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E94" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F94" t="s">
         <v>91</v>
@@ -2814,19 +2814,19 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B95" t="s">
         <v>188</v>
       </c>
       <c r="C95" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D95" t="s">
         <v>69</v>
       </c>
       <c r="E95" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F95" t="s">
         <v>131</v>
@@ -2834,19 +2834,19 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B96" t="s">
         <v>189</v>
       </c>
       <c r="C96" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D96" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E96" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F96" t="s">
         <v>44</v>
@@ -2854,13 +2854,13 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B97" t="s">
         <v>190</v>
       </c>
       <c r="C97" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D97" t="s">
         <v>191</v>
@@ -2874,59 +2874,59 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B98" t="s">
         <v>193</v>
       </c>
       <c r="C98" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D98" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E98" t="s">
         <v>71</v>
       </c>
       <c r="F98" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B99" t="s">
         <v>194</v>
       </c>
       <c r="C99" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D99" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E99" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F99" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B100" t="s">
         <v>195</v>
       </c>
       <c r="C100" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D100" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E100" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F100" t="s">
         <v>79</v>
@@ -2934,13 +2934,13 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B101" t="s">
         <v>196</v>
       </c>
       <c r="C101" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D101" t="s">
         <v>109</v>
@@ -2954,13 +2954,13 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B102" t="s">
         <v>199</v>
       </c>
       <c r="C102" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2969,18 +2969,18 @@
         <v>191</v>
       </c>
       <c r="F102" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B103" t="s">
         <v>200</v>
       </c>
       <c r="C103" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D103" t="s">
         <v>104</v>
@@ -2989,18 +2989,18 @@
         <v>191</v>
       </c>
       <c r="F103" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B104" t="s">
         <v>201</v>
       </c>
       <c r="C104" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D104" t="s">
         <v>197</v>

</xml_diff>